<commit_message>
versao aperfeicoada para 2 tipos de emissao de boletos
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cas\PycharmProjects\automacao_teste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F36CE8D-33AA-414B-90E9-F4955F181618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30B54A8-9D4C-4B52-ADFE-F87666830BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12315" yWindow="5025" windowWidth="38700" windowHeight="15435" xr2:uid="{2E4837B1-E5A9-4898-951A-7984BCF1EA89}"/>
+    <workbookView xWindow="1170" yWindow="2445" windowWidth="21495" windowHeight="15435" xr2:uid="{2E4837B1-E5A9-4898-951A-7984BCF1EA89}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,28 +36,124 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
   <si>
     <t>maxi massas</t>
   </si>
   <si>
-    <t>Cliente</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Valor</t>
-  </si>
-  <si>
-    <t>isabella</t>
+    <t>Casa Deliza AQA/SC</t>
+  </si>
+  <si>
+    <t>Barão Consórcios</t>
+  </si>
+  <si>
+    <t>Shopping Lupo</t>
+  </si>
+  <si>
+    <t>Borsari Imóveis</t>
+  </si>
+  <si>
+    <t>Agrotécnica</t>
+  </si>
+  <si>
+    <t>Animalia Rio Preto</t>
+  </si>
+  <si>
+    <t>Passarinho Hortifrúti</t>
+  </si>
+  <si>
+    <t>Julianeti</t>
+  </si>
+  <si>
+    <t>Micelli</t>
+  </si>
+  <si>
+    <t>Trinity</t>
+  </si>
+  <si>
+    <t>Casa9</t>
+  </si>
+  <si>
+    <t>Spazzeo</t>
+  </si>
+  <si>
+    <t>Hotel Salto Grande</t>
+  </si>
+  <si>
+    <t>Fuba</t>
+  </si>
+  <si>
+    <t>Dental Power</t>
+  </si>
+  <si>
+    <t>Apoio</t>
+  </si>
+  <si>
+    <t>4766441153460561</t>
+  </si>
+  <si>
+    <t>589096946057116</t>
+  </si>
+  <si>
+    <t>350829366163255</t>
+  </si>
+  <si>
+    <t>757419351915951</t>
+  </si>
+  <si>
+    <t>747162889648020</t>
+  </si>
+  <si>
+    <t>477908569850788</t>
+  </si>
+  <si>
+    <t>704083103754311</t>
+  </si>
+  <si>
+    <t>332223135566070</t>
+  </si>
+  <si>
+    <t>866541220063713</t>
+  </si>
+  <si>
+    <t>368957994998298</t>
+  </si>
+  <si>
+    <t>538295984311594</t>
+  </si>
+  <si>
+    <t>690102435386578</t>
+  </si>
+  <si>
+    <t>957297151620080</t>
+  </si>
+  <si>
+    <t>725054975582041</t>
+  </si>
+  <si>
+    <t>1314936005979662</t>
+  </si>
+  <si>
+    <t>1119662528586518</t>
+  </si>
+  <si>
+    <t>618129976369036</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +166,19 @@
       <color rgb="FF808080"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="JetBrains Mono"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,9 +201,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -411,48 +527,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F3DE4B0-EE18-47F5-BA0A-9E1B653640CD}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>704083103754311</v>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C2">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
-        <v>766378280835452</v>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>55</v>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>